<commit_message>
Add new participants 2
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="462">
   <si>
     <t xml:space="preserve">timestamp</t>
   </si>
@@ -1331,6 +1331,81 @@
   </si>
   <si>
     <t xml:space="preserve">B20286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/31/2020 2:54:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20108@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kanchan Padvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/509219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/30/2020 21:24:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20133@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shailesh Rathod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/509167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/31/2020 1:02:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20124@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20124 Rajeev Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/509266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/31/2020 11:46:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20162@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavitra Jain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/509047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/31/2020 13:50:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20097@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIYA ASHISH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/508228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20097</t>
   </si>
 </sst>
 </file>
@@ -1550,15 +1625,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F103" activeCellId="0" sqref="F103"/>
+      <selection pane="bottomLeft" activeCell="E101" activeCellId="0" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.29"/>
@@ -3545,6 +3620,106 @@
       </c>
       <c r="F99" s="8" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="F100" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="E101" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="F103" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3647,6 +3822,11 @@
     <hyperlink ref="D97" r:id="rId96" display="https://www.urionlinejudge.com.br/judge/en/profile/508594"/>
     <hyperlink ref="D98" r:id="rId97" display="https://www.urionlinejudge.com.br/judge/en/profile/508237"/>
     <hyperlink ref="D99" r:id="rId98" display="https://www.urionlinejudge.com.br/judge/en/profile/506725"/>
+    <hyperlink ref="D100" r:id="rId99" display="https://www.urionlinejudge.com.br/judge/en/profile/509219"/>
+    <hyperlink ref="D101" r:id="rId100" display="https://www.urionlinejudge.com.br/judge/en/profile/509167"/>
+    <hyperlink ref="D102" r:id="rId101" display="https://www.urionlinejudge.com.br/judge/en/profile/509266"/>
+    <hyperlink ref="D103" r:id="rId102" display="https://www.urionlinejudge.com.br/judge/en/profile/509047"/>
+    <hyperlink ref="D104" r:id="rId103" display="https://www.urionlinejudge.com.br/judge/en/profile/508228"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add change in points and change footer
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="466">
   <si>
     <t xml:space="preserve">timestamp</t>
   </si>
@@ -1406,15 +1406,28 @@
   </si>
   <si>
     <t xml:space="preserve">B20097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b20314@students.iitmandi.ac.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohan Bharti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.urionlinejudge.com.br/judge/en/profile/508146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20314</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1511,7 +1524,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1545,6 +1558,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1625,15 +1642,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E101" activeCellId="0" sqref="E101"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G101" activeCellId="0" sqref="G101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.29"/>
@@ -3720,6 +3737,26 @@
       </c>
       <c r="F104" s="8" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="9" t="n">
+        <v>44197.0350925926</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3827,6 +3864,7 @@
     <hyperlink ref="D102" r:id="rId101" display="https://www.urionlinejudge.com.br/judge/en/profile/509266"/>
     <hyperlink ref="D103" r:id="rId102" display="https://www.urionlinejudge.com.br/judge/en/profile/509047"/>
     <hyperlink ref="D104" r:id="rId103" display="https://www.urionlinejudge.com.br/judge/en/profile/508228"/>
+    <hyperlink ref="D105" r:id="rId104" display="https://www.urionlinejudge.com.br/judge/en/profile/508146"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>